<commit_message>
add table related files
</commit_message>
<xml_diff>
--- a/scripts/perplexity_tables.xlsx
+++ b/scripts/perplexity_tables.xlsx
@@ -474,7 +474,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>257.39</v>
+        <v>251.43</v>
       </c>
       <c r="C2" t="n">
         <v>260.83</v>
@@ -496,7 +496,7 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>114.17</v>
+        <v>114.1</v>
       </c>
       <c r="C3" t="n">
         <v>129.76</v>
@@ -518,7 +518,7 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>83.84999999999999</v>
+        <v>83.55</v>
       </c>
       <c r="C4" t="n">
         <v>99.61</v>
@@ -540,7 +540,7 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>67.89</v>
+        <v>68.02</v>
       </c>
       <c r="C5" t="n">
         <v>84.45</v>
@@ -562,7 +562,7 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>57.46</v>
+        <v>57.38</v>
       </c>
       <c r="C6" t="n">
         <v>74.67</v>
@@ -584,7 +584,7 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>49.25</v>
+        <v>49.04</v>
       </c>
       <c r="C7" t="n">
         <v>67.75</v>
@@ -606,7 +606,7 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>41.63</v>
+        <v>41.77</v>
       </c>
       <c r="C8" t="n">
         <v>62.18</v>
@@ -628,7 +628,7 @@
         </is>
       </c>
       <c r="B9" t="n">
-        <v>35.29</v>
+        <v>35.51</v>
       </c>
       <c r="C9" t="n">
         <v>57.64</v>
@@ -650,7 +650,7 @@
         </is>
       </c>
       <c r="B10" t="n">
-        <v>30.26</v>
+        <v>30.42</v>
       </c>
       <c r="C10" t="n">
         <v>54.07</v>
@@ -672,7 +672,7 @@
         </is>
       </c>
       <c r="B11" t="n">
-        <v>26.32</v>
+        <v>26.46</v>
       </c>
       <c r="C11" t="n">
         <v>51.49</v>
@@ -694,7 +694,7 @@
         </is>
       </c>
       <c r="B12" t="n">
-        <v>23.02</v>
+        <v>23.28</v>
       </c>
       <c r="C12" t="n">
         <v>48.78</v>
@@ -716,7 +716,7 @@
         </is>
       </c>
       <c r="B13" t="n">
-        <v>20.51</v>
+        <v>20.75</v>
       </c>
       <c r="C13" t="n">
         <v>46.59</v>
@@ -738,7 +738,7 @@
         </is>
       </c>
       <c r="B14" t="n">
-        <v>18.51</v>
+        <v>18.77</v>
       </c>
       <c r="C14" t="n">
         <v>44.59</v>
@@ -760,7 +760,7 @@
         </is>
       </c>
       <c r="B15" t="n">
-        <v>16.94</v>
+        <v>17.23</v>
       </c>
       <c r="C15" t="n">
         <v>43.04</v>
@@ -782,7 +782,7 @@
         </is>
       </c>
       <c r="B16" t="n">
-        <v>15.63</v>
+        <v>16.03</v>
       </c>
       <c r="C16" t="n">
         <v>41.52</v>
@@ -804,7 +804,7 @@
         </is>
       </c>
       <c r="B17" t="n">
-        <v>14.64</v>
+        <v>14.95</v>
       </c>
       <c r="C17" t="n">
         <v>40.18</v>
@@ -826,7 +826,7 @@
         </is>
       </c>
       <c r="B18" t="n">
-        <v>13.77</v>
+        <v>14.09</v>
       </c>
       <c r="C18" t="n">
         <v>39.06</v>
@@ -848,7 +848,7 @@
         </is>
       </c>
       <c r="B19" t="n">
-        <v>13.01</v>
+        <v>13.38</v>
       </c>
       <c r="C19" t="n">
         <v>37.81</v>
@@ -870,7 +870,7 @@
         </is>
       </c>
       <c r="B20" t="n">
-        <v>12.37</v>
+        <v>12.7</v>
       </c>
       <c r="C20" t="n">
         <v>37.11</v>
@@ -892,7 +892,7 @@
         </is>
       </c>
       <c r="B21" t="n">
-        <v>11.81</v>
+        <v>12.07</v>
       </c>
       <c r="C21" t="n">
         <v>36.14</v>
@@ -914,7 +914,7 @@
         </is>
       </c>
       <c r="B22" t="n">
-        <v>11.36</v>
+        <v>11.67</v>
       </c>
       <c r="C22" t="n">
         <v>35.45</v>
@@ -936,7 +936,7 @@
         </is>
       </c>
       <c r="B23" t="n">
-        <v>10.98</v>
+        <v>11.23</v>
       </c>
       <c r="C23" t="n">
         <v>34.81</v>
@@ -958,7 +958,7 @@
         </is>
       </c>
       <c r="B24" t="n">
-        <v>10.69</v>
+        <v>10.89</v>
       </c>
       <c r="C24" t="n">
         <v>34.04</v>
@@ -980,7 +980,7 @@
         </is>
       </c>
       <c r="B25" t="n">
-        <v>10.38</v>
+        <v>10.51</v>
       </c>
       <c r="C25" t="n">
         <v>33.5</v>
@@ -1002,7 +1002,7 @@
         </is>
       </c>
       <c r="B26" t="n">
-        <v>10.18</v>
+        <v>10.31</v>
       </c>
       <c r="C26" t="n">
         <v>32.89</v>
@@ -1024,7 +1024,7 @@
         </is>
       </c>
       <c r="B27" t="n">
-        <v>9.81</v>
+        <v>9.949999999999999</v>
       </c>
       <c r="C27" t="n">
         <v>32.36</v>
@@ -1046,7 +1046,7 @@
         </is>
       </c>
       <c r="B28" t="n">
-        <v>9.609999999999999</v>
+        <v>9.66</v>
       </c>
       <c r="C28" t="n">
         <v>31.82</v>
@@ -1068,7 +1068,7 @@
         </is>
       </c>
       <c r="B29" t="n">
-        <v>9.52</v>
+        <v>9.48</v>
       </c>
       <c r="C29" t="n">
         <v>31.4</v>
@@ -1090,7 +1090,7 @@
         </is>
       </c>
       <c r="B30" t="n">
-        <v>9.210000000000001</v>
+        <v>9.23</v>
       </c>
       <c r="C30" t="n">
         <v>31.11</v>
@@ -1112,7 +1112,7 @@
         </is>
       </c>
       <c r="B31" t="n">
-        <v>9.06</v>
+        <v>9.029999999999999</v>
       </c>
       <c r="C31" t="n">
         <v>30.76</v>
@@ -1134,7 +1134,7 @@
         </is>
       </c>
       <c r="B32" t="n">
-        <v>8.92</v>
+        <v>8.890000000000001</v>
       </c>
       <c r="C32" t="n">
         <v>30.53</v>
@@ -1178,7 +1178,7 @@
         </is>
       </c>
       <c r="B34" t="n">
-        <v>8.609999999999999</v>
+        <v>8.56</v>
       </c>
       <c r="C34" t="n">
         <v>29.85</v>
@@ -1200,7 +1200,7 @@
         </is>
       </c>
       <c r="B35" t="n">
-        <v>8.51</v>
+        <v>8.449999999999999</v>
       </c>
       <c r="C35" t="n">
         <v>24.92</v>
@@ -1222,7 +1222,7 @@
         </is>
       </c>
       <c r="B36" t="n">
-        <v>8.33</v>
+        <v>8.25</v>
       </c>
       <c r="C36" t="n">
         <v>24.12</v>
@@ -1244,7 +1244,7 @@
         </is>
       </c>
       <c r="B37" t="n">
-        <v>8.07</v>
+        <v>8.039999999999999</v>
       </c>
       <c r="C37" t="n">
         <v>23.63</v>
@@ -1266,7 +1266,7 @@
         </is>
       </c>
       <c r="B38" t="n">
-        <v>8.02</v>
+        <v>8.01</v>
       </c>
       <c r="C38" t="n">
         <v>23.04</v>
@@ -1288,7 +1288,7 @@
         </is>
       </c>
       <c r="B39" t="n">
-        <v>5.43</v>
+        <v>7.89</v>
       </c>
       <c r="C39" t="n">
         <v>22.8</v>
@@ -1310,7 +1310,7 @@
         </is>
       </c>
       <c r="B40" t="n">
-        <v>4.31</v>
+        <v>7.75</v>
       </c>
       <c r="C40" t="n">
         <v>22.58</v>
@@ -1332,7 +1332,7 @@
         </is>
       </c>
       <c r="B41" t="n">
-        <v>3.73</v>
+        <v>5.28</v>
       </c>
       <c r="C41" t="n">
         <v>22.36</v>
@@ -1405,7 +1405,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>174.27</v>
+        <v>186.16</v>
       </c>
       <c r="C2" t="n">
         <v>165.24</v>
@@ -1427,7 +1427,7 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>97.09</v>
+        <v>96.17</v>
       </c>
       <c r="C3" t="n">
         <v>101.9</v>
@@ -1449,7 +1449,7 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>75.08</v>
+        <v>78.86</v>
       </c>
       <c r="C4" t="n">
         <v>82.12</v>
@@ -1471,7 +1471,7 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>62.87</v>
+        <v>65.72</v>
       </c>
       <c r="C5" t="n">
         <v>69.79000000000001</v>
@@ -1493,7 +1493,7 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>53.47</v>
+        <v>53.86</v>
       </c>
       <c r="C6" t="n">
         <v>61.21</v>
@@ -1515,7 +1515,7 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>46.53</v>
+        <v>46.37</v>
       </c>
       <c r="C7" t="n">
         <v>55.14</v>
@@ -1537,7 +1537,7 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>40.44</v>
+        <v>40.28</v>
       </c>
       <c r="C8" t="n">
         <v>49.76</v>
@@ -1559,7 +1559,7 @@
         </is>
       </c>
       <c r="B9" t="n">
-        <v>35.8</v>
+        <v>34.59</v>
       </c>
       <c r="C9" t="n">
         <v>45.93</v>
@@ -1581,7 +1581,7 @@
         </is>
       </c>
       <c r="B10" t="n">
-        <v>31.57</v>
+        <v>30.43</v>
       </c>
       <c r="C10" t="n">
         <v>42.63</v>
@@ -1603,7 +1603,7 @@
         </is>
       </c>
       <c r="B11" t="n">
-        <v>27.95</v>
+        <v>27.74</v>
       </c>
       <c r="C11" t="n">
         <v>39.69</v>
@@ -1625,7 +1625,7 @@
         </is>
       </c>
       <c r="B12" t="n">
-        <v>25.27</v>
+        <v>24.92</v>
       </c>
       <c r="C12" t="n">
         <v>36.72</v>
@@ -1647,7 +1647,7 @@
         </is>
       </c>
       <c r="B13" t="n">
-        <v>23.4</v>
+        <v>22.58</v>
       </c>
       <c r="C13" t="n">
         <v>34.54</v>
@@ -1669,7 +1669,7 @@
         </is>
       </c>
       <c r="B14" t="n">
-        <v>21.31</v>
+        <v>21.06</v>
       </c>
       <c r="C14" t="n">
         <v>32.56</v>
@@ -1691,7 +1691,7 @@
         </is>
       </c>
       <c r="B15" t="n">
-        <v>19.69</v>
+        <v>19.66</v>
       </c>
       <c r="C15" t="n">
         <v>30.99</v>
@@ -1713,7 +1713,7 @@
         </is>
       </c>
       <c r="B16" t="n">
-        <v>18.26</v>
+        <v>18.11</v>
       </c>
       <c r="C16" t="n">
         <v>29.15</v>
@@ -1735,7 +1735,7 @@
         </is>
       </c>
       <c r="B17" t="n">
-        <v>16.97</v>
+        <v>16.77</v>
       </c>
       <c r="C17" t="n">
         <v>27.81</v>
@@ -1757,7 +1757,7 @@
         </is>
       </c>
       <c r="B18" t="n">
-        <v>16.22</v>
+        <v>16.07</v>
       </c>
       <c r="C18" t="n">
         <v>26.67</v>
@@ -1779,7 +1779,7 @@
         </is>
       </c>
       <c r="B19" t="n">
-        <v>15.09</v>
+        <v>15.24</v>
       </c>
       <c r="C19" t="n">
         <v>25.56</v>
@@ -1801,7 +1801,7 @@
         </is>
       </c>
       <c r="B20" t="n">
-        <v>14.54</v>
+        <v>14.38</v>
       </c>
       <c r="C20" t="n">
         <v>24.51</v>
@@ -1823,7 +1823,7 @@
         </is>
       </c>
       <c r="B21" t="n">
-        <v>14.22</v>
+        <v>13.62</v>
       </c>
       <c r="C21" t="n">
         <v>23.37</v>
@@ -1845,7 +1845,7 @@
         </is>
       </c>
       <c r="B22" t="n">
-        <v>13.29</v>
+        <v>12.85</v>
       </c>
       <c r="C22" t="n">
         <v>22.98</v>
@@ -1867,7 +1867,7 @@
         </is>
       </c>
       <c r="B23" t="n">
-        <v>12.91</v>
+        <v>12.14</v>
       </c>
       <c r="C23" t="n">
         <v>21.78</v>
@@ -1889,7 +1889,7 @@
         </is>
       </c>
       <c r="B24" t="n">
-        <v>12.33</v>
+        <v>11.6</v>
       </c>
       <c r="C24" t="n">
         <v>21.29</v>
@@ -1911,7 +1911,7 @@
         </is>
       </c>
       <c r="B25" t="n">
-        <v>11.8</v>
+        <v>11.17</v>
       </c>
       <c r="C25" t="n">
         <v>20.27</v>
@@ -1933,7 +1933,7 @@
         </is>
       </c>
       <c r="B26" t="n">
-        <v>11.19</v>
+        <v>10.87</v>
       </c>
       <c r="C26" t="n">
         <v>19.92</v>
@@ -1955,7 +1955,7 @@
         </is>
       </c>
       <c r="B27" t="n">
-        <v>10.79</v>
+        <v>10.68</v>
       </c>
       <c r="C27" t="n">
         <v>19.49</v>
@@ -1977,7 +1977,7 @@
         </is>
       </c>
       <c r="B28" t="n">
-        <v>10.56</v>
+        <v>10.25</v>
       </c>
       <c r="C28" t="n">
         <v>19.02</v>
@@ -1999,7 +1999,7 @@
         </is>
       </c>
       <c r="B29" t="n">
-        <v>10.18</v>
+        <v>9.93</v>
       </c>
       <c r="C29" t="n">
         <v>18.36</v>
@@ -2021,7 +2021,7 @@
         </is>
       </c>
       <c r="B30" t="n">
-        <v>9.67</v>
+        <v>9.58</v>
       </c>
       <c r="C30" t="n">
         <v>18.09</v>
@@ -2043,7 +2043,7 @@
         </is>
       </c>
       <c r="B31" t="n">
-        <v>9.460000000000001</v>
+        <v>9.31</v>
       </c>
       <c r="C31" t="n">
         <v>17.6</v>
@@ -2065,7 +2065,7 @@
         </is>
       </c>
       <c r="B32" t="n">
-        <v>9.140000000000001</v>
+        <v>9.130000000000001</v>
       </c>
       <c r="C32" t="n">
         <v>17.47</v>
@@ -2087,7 +2087,7 @@
         </is>
       </c>
       <c r="B33" t="n">
-        <v>8.99</v>
+        <v>8.779999999999999</v>
       </c>
       <c r="C33" t="n">
         <v>16.84</v>
@@ -2109,7 +2109,7 @@
         </is>
       </c>
       <c r="B34" t="n">
-        <v>8.82</v>
+        <v>8.640000000000001</v>
       </c>
       <c r="C34" t="n">
         <v>16.9</v>
@@ -2131,7 +2131,7 @@
         </is>
       </c>
       <c r="B35" t="n">
-        <v>8.789999999999999</v>
+        <v>8.41</v>
       </c>
       <c r="C35" t="n">
         <v>14.53</v>
@@ -2153,7 +2153,7 @@
         </is>
       </c>
       <c r="B36" t="n">
-        <v>8.4</v>
+        <v>8.24</v>
       </c>
       <c r="C36" t="n">
         <v>14</v>
@@ -2175,7 +2175,7 @@
         </is>
       </c>
       <c r="B37" t="n">
-        <v>8.029999999999999</v>
+        <v>8.09</v>
       </c>
       <c r="C37" t="n">
         <v>13.56</v>
@@ -2197,7 +2197,7 @@
         </is>
       </c>
       <c r="B38" t="n">
-        <v>8.039999999999999</v>
+        <v>7.81</v>
       </c>
       <c r="C38" t="n">
         <v>13.3</v>
@@ -2219,7 +2219,7 @@
         </is>
       </c>
       <c r="B39" t="n">
-        <v>5.22</v>
+        <v>7.69</v>
       </c>
       <c r="C39" t="n">
         <v>12.98</v>
@@ -2241,7 +2241,7 @@
         </is>
       </c>
       <c r="B40" t="n">
-        <v>4.51</v>
+        <v>7.71</v>
       </c>
       <c r="C40" t="n">
         <v>12.74</v>
@@ -2263,7 +2263,7 @@
         </is>
       </c>
       <c r="B41" t="n">
-        <v>4.06</v>
+        <v>5.03</v>
       </c>
       <c r="C41" t="n">
         <v>12.52</v>
@@ -2336,7 +2336,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>4.32</v>
+        <v>5.29</v>
       </c>
       <c r="C2" t="n">
         <v>13.37</v>

</xml_diff>